<commit_message>
feat(anidb_article): articleDto with upvotes and Paging test complete.
* article mapper and related files added and modified.
Now can get
    * Paging
    * ArticleDTo
</commit_message>
<xml_diff>
--- a/src/main/resources/API/api_prototype.xlsx
+++ b/src/main/resources/API/api_prototype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\cms\spring-projects\aniDB\aniDB_backend\src\main\resources\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94624A2-915A-4B26-9797-3D3B80C62C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C4D83-BC75-4542-A2BC-72C2139B9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +288,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,8 +313,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -315,8 +327,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -324,17 +351,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="나쁨" xfId="2" builtinId="27"/>
+    <cellStyle name="메모" xfId="3" builtinId="10"/>
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -614,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -658,71 +693,71 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -745,25 +780,25 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -844,25 +879,25 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -901,71 +936,71 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -973,11 +1008,11 @@
       <c r="C21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
@@ -986,7 +1021,7 @@
       <c r="E22" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22" t="s">
@@ -994,107 +1029,161 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
feat(upvote comment): upvoting comment API added.
* POST
* DELETE
</commit_message>
<xml_diff>
--- a/src/main/resources/API/api_prototype.xlsx
+++ b/src/main/resources/API/api_prototype.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\cms\spring-projects\aniDB\aniDB_backend\src\main\resources\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C4D83-BC75-4542-A2BC-72C2139B9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7EDD67-524F-4D69-A904-2B9764C4B7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>Method</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -250,6 +250,22 @@
   </si>
   <si>
     <t>PublicationDTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>upvote/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/article/{articleId}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comment/{commentId}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/publication/{publicationId}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -649,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1185,6 +1201,54 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>